<commit_message>
Cambios en archivos de Data/Raw
</commit_message>
<xml_diff>
--- a/data/raw/electrica_25.xlsx
+++ b/data/raw/electrica_25.xlsx
@@ -1,80 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Oscar\Projects\data-INSCO-hub\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECC5650-6B77-4898-B053-5C6378D9DCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="104">
-  <si>
-    <t>NUMERO DE INFORME</t>
-  </si>
-  <si>
-    <t>Orden de Servicio</t>
-  </si>
-  <si>
-    <t>Asignados</t>
-  </si>
-  <si>
-    <t>CALIBRADO POR</t>
-  </si>
-  <si>
-    <t>SUPERVISADO POR</t>
-  </si>
-  <si>
-    <t>APROBADO POR</t>
-  </si>
-  <si>
-    <t>CLASIFICACIÓN</t>
-  </si>
-  <si>
-    <t>FECHA DE RECEPCIÓN A LAB</t>
-  </si>
-  <si>
-    <t>FECHA PROGRAMADA DE ENTREGA</t>
-  </si>
-  <si>
-    <t>FECHA DE LIMPIEZA</t>
-  </si>
-  <si>
-    <t>FECHA DE CALIBRACIÓN</t>
-  </si>
-  <si>
-    <t>FECHA DE ENTREGA</t>
-  </si>
-  <si>
-    <t>TIEMPO DE ENTREGA</t>
-  </si>
-  <si>
-    <t>ESTATUS LAB</t>
-  </si>
-  <si>
-    <t>TIEMPO ASIGNADO</t>
-  </si>
-  <si>
-    <t>SERVICIO EN</t>
-  </si>
-  <si>
-    <t>MOTIVO DE SUSTITUCIÓN DE INFORME</t>
-  </si>
-  <si>
-    <t>OBSERVACIÓNES LAB</t>
-  </si>
-  <si>
-    <t>URGENCIA DEL SERVICIO</t>
-  </si>
-  <si>
-    <t>NÚMERO DE PIEZAS</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="103">
   <si>
     <t>CCM0001.E/2025</t>
   </si>
@@ -271,9 +217,6 @@
     <t>I0357</t>
   </si>
   <si>
-    <t>María G. Rodríguez Suárez</t>
-  </si>
-  <si>
     <t>CCM0026.E/2025</t>
   </si>
   <si>
@@ -326,16 +269,76 @@
   </si>
   <si>
     <t>H2492</t>
+  </si>
+  <si>
+    <t>report_number</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>assignee</t>
+  </si>
+  <si>
+    <t>calibrator</t>
+  </si>
+  <si>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>approver</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>lab_received_date</t>
+  </si>
+  <si>
+    <t>scheduled_delivery_date</t>
+  </si>
+  <si>
+    <t>cleaning_date</t>
+  </si>
+  <si>
+    <t>calibration_date</t>
+  </si>
+  <si>
+    <t>delivery_date</t>
+  </si>
+  <si>
+    <t>delivery_time</t>
+  </si>
+  <si>
+    <t>process_status</t>
+  </si>
+  <si>
+    <t>assigned_time</t>
+  </si>
+  <si>
+    <t>service_location</t>
+  </si>
+  <si>
+    <t>substitution_reason</t>
+  </si>
+  <si>
+    <t>lab_observations</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>piece_count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -386,14 +389,24 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{53B8D8B8-3BFE-4479-B44C-B7B18ECF98F5}"/>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -431,7 +444,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -465,6 +478,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -499,9 +513,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -674,99 +689,101 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:T35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="R3" sqref="R3:R6 R8:R24 R26:R30 J2:J34 R33:R34 A35:T35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="20" width="30.7109375" customWidth="1"/>
+    <col min="1" max="20" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="H2" s="3">
         <v>45653</v>
@@ -785,48 +802,48 @@
         <v>16</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O2" s="2">
         <v>19</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T2" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="H3" s="3">
         <v>45665</v>
@@ -845,46 +862,46 @@
         <v>12</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O3" s="2">
         <v>13</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R3" s="2"/>
       <c r="S3" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H4" s="3">
         <v>45666</v>
@@ -903,46 +920,46 @@
         <v>11</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O4" s="2">
         <v>13</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R4" s="2"/>
       <c r="S4" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T4" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3">
         <v>45670</v>
@@ -961,46 +978,46 @@
         <v>2</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O5" s="2">
         <v>3</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q5" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R5" s="2"/>
       <c r="S5" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T5" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H6" s="3">
         <v>45671</v>
@@ -1019,46 +1036,46 @@
         <v>12</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O6" s="2">
         <v>13</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R6" s="2"/>
       <c r="S6" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T6" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H7" s="3">
         <v>45672</v>
@@ -1077,48 +1094,48 @@
         <v>16</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O7" s="2">
         <v>17</v>
       </c>
       <c r="P7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20">
-      <c r="A8" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>46</v>
-      </c>
       <c r="C8" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H8" s="3">
         <v>45673</v>
@@ -1137,46 +1154,46 @@
         <v>10</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O8" s="2">
         <v>13</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T8" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H9" s="3">
         <v>45677</v>
@@ -1195,46 +1212,46 @@
         <v>8</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O9" s="2">
         <v>13</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="T9" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H10" s="3">
         <v>45679</v>
@@ -1253,46 +1270,46 @@
         <v>8</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O10" s="2">
         <v>13</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T10" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H11" s="3">
         <v>45680</v>
@@ -1311,46 +1328,46 @@
         <v>10</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O11" s="2">
         <v>13</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T11" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:20">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H12" s="3">
         <v>45688</v>
@@ -1369,46 +1386,46 @@
         <v>12</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O12" s="2">
         <v>13</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R12" s="2"/>
       <c r="S12" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T12" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="H13" s="3">
         <v>45688</v>
@@ -1427,46 +1444,46 @@
         <v>7</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O13" s="2">
         <v>13</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R13" s="2"/>
       <c r="S13" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T13" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H14" s="3">
         <v>45692</v>
@@ -1485,46 +1502,46 @@
         <v>11</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O14" s="2">
         <v>13</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R14" s="2"/>
       <c r="S14" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T14" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H15" s="3">
         <v>45693</v>
@@ -1543,46 +1560,46 @@
         <v>11</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O15" s="2">
         <v>13</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R15" s="2"/>
       <c r="S15" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H16" s="3">
         <v>45698</v>
@@ -1601,46 +1618,46 @@
         <v>13</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O16" s="2">
         <v>13</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R16" s="2"/>
       <c r="S16" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T16" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H17" s="3">
         <v>45709</v>
@@ -1659,46 +1676,46 @@
         <v>7</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O17" s="2">
         <v>17</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R17" s="2"/>
       <c r="S17" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T17" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H18" s="3">
         <v>45712</v>
@@ -1717,46 +1734,46 @@
         <v>4</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O18" s="2">
         <v>13</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R18" s="2"/>
       <c r="S18" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T18" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H19" s="3">
         <v>45712</v>
@@ -1775,46 +1792,46 @@
         <v>7</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O19" s="2">
         <v>13</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R19" s="2"/>
       <c r="S19" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T19" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H20" s="3">
         <v>45714</v>
@@ -1833,46 +1850,46 @@
         <v>5</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O20" s="2">
         <v>13</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T20" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H21" s="3">
         <v>45715</v>
@@ -1891,46 +1908,46 @@
         <v>15</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O21" s="2">
         <v>17</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R21" s="2"/>
       <c r="S21" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T21" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H22" s="3">
         <v>45716</v>
@@ -1949,46 +1966,46 @@
         <v>4</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O22" s="2">
         <v>13</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q22" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R22" s="2"/>
       <c r="S22" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T22" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H23" s="3">
         <v>45719</v>
@@ -2007,46 +2024,46 @@
         <v>3</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O23" s="2">
         <v>13</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R23" s="2"/>
       <c r="S23" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T23" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H24" s="3">
         <v>45720</v>
@@ -2065,46 +2082,46 @@
         <v>10</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O24" s="2">
         <v>13</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R24" s="2"/>
       <c r="S24" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T24" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H25" s="3">
         <v>45720</v>
@@ -2123,48 +2140,48 @@
         <v>2</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O25" s="2">
         <v>13</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R25" s="2" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="S25" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T25" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H26" s="3">
         <v>45721</v>
@@ -2183,368 +2200,404 @@
         <v>1</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O26" s="2">
         <v>13</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R26" s="2"/>
       <c r="S26" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T26" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="C27" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="H27" s="3">
+        <v>45723</v>
+      </c>
+      <c r="I27" s="3">
+        <v>45743</v>
+      </c>
       <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
-      <c r="N27" s="2"/>
-      <c r="O27" s="2"/>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2"/>
+      <c r="K27" s="3">
+        <v>45737</v>
+      </c>
+      <c r="L27" s="3">
+        <v>45740</v>
+      </c>
+      <c r="M27" s="2">
+        <v>10</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O27" s="2">
+        <v>13</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="R27" s="2"/>
-      <c r="S27" s="2"/>
-      <c r="T27" s="2"/>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="S27" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T27" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>87</v>
+        <v>68</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H28" s="3">
-        <v>45723</v>
+        <v>45726</v>
       </c>
       <c r="I28" s="3">
-        <v>45743</v>
+        <v>45744</v>
       </c>
       <c r="J28" s="2"/>
       <c r="K28" s="3">
-        <v>45737</v>
+        <v>45740</v>
       </c>
       <c r="L28" s="3">
-        <v>45740</v>
+        <v>45741</v>
       </c>
       <c r="M28" s="2">
         <v>10</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O28" s="2">
         <v>13</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R28" s="2"/>
       <c r="S28" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T28" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H29" s="3">
-        <v>45726</v>
+        <v>45727</v>
       </c>
       <c r="I29" s="3">
-        <v>45744</v>
+        <v>45747</v>
       </c>
       <c r="J29" s="2"/>
       <c r="K29" s="3">
-        <v>45740</v>
+        <v>45742</v>
       </c>
       <c r="L29" s="3">
-        <v>45741</v>
+        <v>45743</v>
       </c>
       <c r="M29" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O29" s="2">
         <v>13</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T29" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="H30" s="3">
-        <v>45727</v>
+        <v>45728</v>
       </c>
       <c r="I30" s="3">
-        <v>45747</v>
+        <v>45748</v>
       </c>
       <c r="J30" s="2"/>
       <c r="K30" s="3">
-        <v>45742</v>
+        <v>45744</v>
       </c>
       <c r="L30" s="3">
-        <v>45743</v>
+        <v>45747</v>
       </c>
       <c r="M30" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O30" s="2">
         <v>13</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q30" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T30" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="H31" s="3">
-        <v>45728</v>
+        <v>45635</v>
       </c>
       <c r="I31" s="3">
-        <v>45748</v>
+        <v>45674</v>
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="3">
-        <v>45744</v>
+        <v>45673</v>
       </c>
       <c r="L31" s="3">
-        <v>45747</v>
+        <v>45673</v>
       </c>
       <c r="M31" s="2">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O31" s="2">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R31" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="R31" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="S31" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T31" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="H32" s="3">
-        <v>45635</v>
+        <v>45637</v>
       </c>
       <c r="I32" s="3">
-        <v>45674</v>
+        <v>45671</v>
       </c>
       <c r="J32" s="2"/>
       <c r="K32" s="3">
-        <v>45673</v>
+        <v>45668</v>
       </c>
       <c r="L32" s="3">
-        <v>45673</v>
+        <v>45671</v>
       </c>
       <c r="M32" s="2">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O32" s="2">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="S32" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T32" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H33" s="3">
-        <v>45637</v>
+        <v>45643</v>
       </c>
       <c r="I33" s="3">
-        <v>45671</v>
+        <v>45672</v>
       </c>
       <c r="J33" s="2"/>
       <c r="K33" s="3">
@@ -2554,143 +2607,83 @@
         <v>45671</v>
       </c>
       <c r="M33" s="2">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O33" s="2">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R33" s="2" t="s">
-        <v>99</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="R33" s="2"/>
       <c r="S33" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T33" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H34" s="3">
-        <v>45643</v>
+        <v>45646</v>
       </c>
       <c r="I34" s="3">
-        <v>45672</v>
+        <v>45684</v>
       </c>
       <c r="J34" s="2"/>
       <c r="K34" s="3">
-        <v>45668</v>
+        <v>45678</v>
       </c>
       <c r="L34" s="3">
-        <v>45671</v>
+        <v>45680</v>
       </c>
       <c r="M34" s="2">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="O34" s="2">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="Q34" s="2" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="R34" s="2"/>
       <c r="S34" s="2" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="T34" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20">
-      <c r="A35" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H35" s="3">
-        <v>45646</v>
-      </c>
-      <c r="I35" s="3">
-        <v>45684</v>
-      </c>
-      <c r="J35" s="2"/>
-      <c r="K35" s="3">
-        <v>45678</v>
-      </c>
-      <c r="L35" s="3">
-        <v>45680</v>
-      </c>
-      <c r="M35" s="2">
-        <v>22</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O35" s="2">
-        <v>24</v>
-      </c>
-      <c r="P35" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q35" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R35" s="2"/>
-      <c r="S35" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="T35" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>